<commit_message>
Deleted copy files. Updated template.xlsx
</commit_message>
<xml_diff>
--- a/v2/template.xlsx
+++ b/v2/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akha/Documents/Documents/excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akha/Documents/api_excel/v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3DDB97-DC56-8D4C-BC99-1BDB5FBCA93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458D63B8-3DA4-2F47-92F5-A056072882B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" tabRatio="505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REESTR" sheetId="1" r:id="rId1"/>
@@ -366,9 +366,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#\ ##0.00"/>
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -886,9 +885,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -896,6 +892,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1303,8 +1302,8 @@
   </sheetPr>
   <dimension ref="A1:R322"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1469,12 +1468,12 @@
       <c r="F10" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="77"/>
+      <c r="G10" s="81"/>
       <c r="H10" s="71"/>
       <c r="I10" s="70"/>
       <c r="J10" s="29"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="80"/>
       <c r="M10" s="29"/>
     </row>
     <row r="11" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -1483,12 +1482,12 @@
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
-      <c r="F11" s="78" t="s">
+      <c r="F11" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="80"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="79"/>
     </row>
     <row r="12" spans="1:13" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29"/>
@@ -5241,7 +5240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:K49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6136,8 +6135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A4:N63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6319,6 +6318,30 @@
       <c r="B11" s="25" t="s">
         <v>72</v>
       </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1">
+        <v>7</v>
+      </c>
+      <c r="I11" s="1">
+        <v>8</v>
+      </c>
+      <c r="J11" s="1">
+        <v>9</v>
+      </c>
+      <c r="K11" s="1">
+        <v>10</v>
+      </c>
       <c r="N11" s="1">
         <v>3</v>
       </c>
@@ -6328,6 +6351,30 @@
       <c r="B12" s="25" t="s">
         <v>73</v>
       </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5</v>
+      </c>
+      <c r="G12" s="1">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1">
+        <v>7</v>
+      </c>
+      <c r="I12" s="1">
+        <v>8</v>
+      </c>
+      <c r="J12" s="1">
+        <v>9</v>
+      </c>
+      <c r="K12" s="1">
+        <v>10</v>
+      </c>
       <c r="N12" s="1">
         <v>3</v>
       </c>
@@ -6682,19 +6729,19 @@
       <c r="E24" s="1">
         <v>2</v>
       </c>
+      <c r="F24" s="1">
+        <v>6</v>
+      </c>
       <c r="G24" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H24" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I24" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J24" s="1">
-        <v>9</v>
-      </c>
-      <c r="K24" s="1">
         <v>10</v>
       </c>
       <c r="N24" s="1">
@@ -6712,19 +6759,19 @@
       <c r="E25" s="1">
         <v>2</v>
       </c>
+      <c r="F25" s="1">
+        <v>6</v>
+      </c>
       <c r="G25" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H25" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I25" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J25" s="1">
-        <v>9</v>
-      </c>
-      <c r="K25" s="1">
         <v>10</v>
       </c>
       <c r="N25" s="1">
@@ -6773,14 +6820,30 @@
         <v>87</v>
       </c>
       <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="66"/>
+      <c r="D27" s="67">
+        <v>1</v>
+      </c>
+      <c r="E27" s="67">
+        <v>2</v>
+      </c>
+      <c r="F27" s="67">
+        <v>5</v>
+      </c>
+      <c r="G27" s="67">
+        <v>6</v>
+      </c>
+      <c r="H27" s="67">
+        <v>7</v>
+      </c>
+      <c r="I27" s="67">
+        <v>8</v>
+      </c>
+      <c r="J27" s="67">
+        <v>9</v>
+      </c>
+      <c r="K27" s="67">
+        <v>10</v>
+      </c>
       <c r="L27" s="66"/>
       <c r="M27" s="66"/>
       <c r="N27" s="67">
@@ -7127,7 +7190,6 @@
       <c r="B63" s="28"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="95WvQemOQ7pw8OIdpJA9L822Ul4hIWudL68YB7qZqY5cRxB94bnR3t54X6q36yT9cl4EpRHLc51VuRgQeiqrSQ==" saltValue="a1sQnCng06YiJ00NBFUemg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>

</xml_diff>